<commit_message>
get and post api
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\ICANIO\excelmoduleDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\ICANIO\PRO\excelmoduleDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A44DC2-4917-41D1-B7B8-51E70FBBFAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CDC0E4-37EE-455A-A4A3-47E7C3D792F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01EF61E1-168E-4A18-82E1-2E76F7AE79C9}"/>
   </bookViews>
@@ -782,7 +782,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>